<commit_message>
fixing for both Oracle and Mysql
</commit_message>
<xml_diff>
--- a/TableMetadata/Metadata_MySQL.xlsx
+++ b/TableMetadata/Metadata_MySQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\TableMetadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3110540-8857-445E-888D-9FFEF87371B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A750CA2D-97EA-4C2F-A307-2E5EA8CC2C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>COULMN_NAME</t>
   </si>
@@ -47,9 +47,6 @@
     <t>DEPT</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>varchar</t>
   </si>
   <si>
@@ -62,15 +59,6 @@
     <t>varchar(9)</t>
   </si>
   <si>
-    <t>decimal(4,0)</t>
-  </si>
-  <si>
-    <t>decimal(7,2)</t>
-  </si>
-  <si>
-    <t>decimal(2,0)</t>
-  </si>
-  <si>
     <t>varchar(14)</t>
   </si>
   <si>
@@ -105,6 +93,9 @@
   </si>
   <si>
     <t>comm</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -495,7 +486,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,90 +509,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +605,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,35 +628,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamically added Oracle and Mysql folder under each test case
</commit_message>
<xml_diff>
--- a/TableMetadata/Metadata_MySQL.xlsx
+++ b/TableMetadata/Metadata_MySQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\TableMetadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A750CA2D-97EA-4C2F-A307-2E5EA8CC2C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A610D2-8002-4CDA-900F-ABF672CBA515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added STUDENT table testcase
</commit_message>
<xml_diff>
--- a/TableMetadata/Metadata_MySQL.xlsx
+++ b/TableMetadata/Metadata_MySQL.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\TableMetadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A610D2-8002-4CDA-900F-ABF672CBA515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4528937-6DF5-4349-AD70-61E4E0E3038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_NAMES" sheetId="1" r:id="rId1"/>
     <sheet name="EMP" sheetId="3" r:id="rId2"/>
     <sheet name="DEPT" sheetId="2" r:id="rId3"/>
+    <sheet name="STUDENT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>COULMN_NAME</t>
   </si>
@@ -96,6 +97,27 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>STUDENT</t>
+  </si>
+  <si>
+    <t>Student_id</t>
+  </si>
+  <si>
+    <t>Student_name</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
   </si>
 </sst>
 </file>
@@ -450,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33069F73-A7F6-4D4D-8E2D-2B03998EE77C}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,6 +498,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -485,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFDE1AC-0A85-43BB-9147-181A7311A598}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +539,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -605,7 +632,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,4 +689,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBF71A8-BDA5-4BAF-A9CB-A8AB37D301C3}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added T_EMP table testcases
</commit_message>
<xml_diff>
--- a/TableMetadata/Metadata_MySQL.xlsx
+++ b/TableMetadata/Metadata_MySQL.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\TableMetadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4528937-6DF5-4349-AD70-61E4E0E3038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AFA56B-7816-4992-A327-5EE398453DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{329CFC19-3AC1-4FDD-9D4F-5E2ED556CDD9}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_NAMES" sheetId="1" r:id="rId1"/>
     <sheet name="EMP" sheetId="3" r:id="rId2"/>
     <sheet name="DEPT" sheetId="2" r:id="rId3"/>
     <sheet name="STUDENT" sheetId="4" r:id="rId4"/>
+    <sheet name="T_EMP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
   <si>
     <t>COULMN_NAME</t>
   </si>
@@ -118,6 +119,54 @@
   </si>
   <si>
     <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>JOB_TYPE</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>HIRE_DATE</t>
+  </si>
+  <si>
+    <t>TOTAL_EXP_IN_COMPANY</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>COMMISSION</t>
+  </si>
+  <si>
+    <t>TOTAL_SALARY</t>
+  </si>
+  <si>
+    <t>SALARY_GRADE</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>T_EMP</t>
+  </si>
+  <si>
+    <t>T_EMP_ID</t>
+  </si>
+  <si>
+    <t>EMP_ID</t>
+  </si>
+  <si>
+    <t>EMP_NAME</t>
+  </si>
+  <si>
+    <t>DEPT_NAME</t>
+  </si>
+  <si>
+    <t>MANAGER_NAME</t>
   </si>
 </sst>
 </file>
@@ -472,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33069F73-A7F6-4D4D-8E2D-2B03998EE77C}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,6 +550,11 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -695,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBF71A8-BDA5-4BAF-A9CB-A8AB37D301C3}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,4 +829,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94626991-3F81-4AFF-B64F-D0BD60017DBD}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>